<commit_message>
Trials to avoide compilation error
</commit_message>
<xml_diff>
--- a/Test_Data/Validate_Dulicates.xlsx
+++ b/Test_Data/Validate_Dulicates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ajay\Java_Folder\Java_Eclips\vTiger\Test_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0694438-A8FC-4341-B747-0A4820BA8B40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4EED3ED-6D13-42CE-B034-19B6662AB1F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,6 +63,21 @@
     <t>Other</t>
   </si>
   <si>
+    <t>Abcd</t>
+  </si>
+  <si>
+    <t>xyz</t>
+  </si>
+  <si>
+    <t>Pqr</t>
+  </si>
+  <si>
+    <t>lmn</t>
+  </si>
+  <si>
+    <t>Humar</t>
+  </si>
+  <si>
     <t>January</t>
   </si>
   <si>
@@ -76,21 +91,6 @@
   </si>
   <si>
     <t>May</t>
-  </si>
-  <si>
-    <t>Abcd</t>
-  </si>
-  <si>
-    <t>xyz</t>
-  </si>
-  <si>
-    <t>Pqr</t>
-  </si>
-  <si>
-    <t>lmn</t>
-  </si>
-  <si>
-    <t>Humar</t>
   </si>
 </sst>
 </file>
@@ -417,7 +417,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -452,16 +452,16 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
       <c r="D2">
-        <v>2000</v>
+        <v>1990</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F2">
         <v>10</v>
@@ -472,7 +472,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -481,7 +481,7 @@
         <v>1990</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F3">
         <v>11</v>
@@ -492,16 +492,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
       </c>
       <c r="D4">
-        <v>1995</v>
+        <v>1990</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F4">
         <v>12</v>
@@ -509,19 +509,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
       </c>
       <c r="D5">
-        <v>1998</v>
+        <v>1990</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F5">
         <v>15</v>
@@ -532,16 +532,16 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
       </c>
       <c r="D6">
-        <v>2003</v>
+        <v>1990</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F6">
         <v>18</v>
@@ -550,5 +550,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>